<commit_message>
added dateAdded to datasets.xlsx
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhbertram/Documents/GitHub/TrioSphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B093EB2-A905-0747-9BD3-05F971E9F37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A280261-3C2C-B04F-962A-54FF60BC5430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20980" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="273">
   <si>
     <t>id</t>
   </si>
@@ -1424,6 +1424,9 @@
       <t>&gt;</t>
     </r>
   </si>
+  <si>
+    <t>dateAdded</t>
+  </si>
 </sst>
 </file>
 
@@ -1611,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1634,7 +1637,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,7 +1667,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1721,7 +1724,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1744,6 +1747,9 @@
     </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1971,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2033,7 +2039,9 @@
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2087,7 +2095,9 @@
       <c r="M2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="45">
+        <v>45974</v>
+      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -2141,7 +2151,9 @@
       <c r="M3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="45">
+        <v>45974</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -2197,7 +2209,9 @@
       <c r="M4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="45">
+        <v>45974</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -2251,7 +2265,9 @@
       <c r="M5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="45">
+        <v>45974</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -2305,7 +2321,9 @@
       <c r="M6" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="1"/>
+      <c r="N6" s="45">
+        <v>45974</v>
+      </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -2359,7 +2377,9 @@
       <c r="M7" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="1"/>
+      <c r="N7" s="45">
+        <v>45974</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -2413,7 +2433,9 @@
       <c r="M8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="1"/>
+      <c r="N8" s="45">
+        <v>45974</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -2467,7 +2489,9 @@
       <c r="M9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="45">
+        <v>45974</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -2521,7 +2545,9 @@
       <c r="M10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="45">
+        <v>45974</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -2575,7 +2601,9 @@
       <c r="M11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="45">
+        <v>45974</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -2629,7 +2657,9 @@
       <c r="M12" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="45">
+        <v>45974</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -2683,7 +2713,9 @@
       <c r="M13" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="45">
+        <v>45974</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -2737,7 +2769,9 @@
       <c r="M14" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="45">
+        <v>45974</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -2791,7 +2825,9 @@
       <c r="M15" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="45">
+        <v>45974</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -2845,7 +2881,9 @@
       <c r="M16" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="45">
+        <v>45974</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -2899,7 +2937,9 @@
       <c r="M17" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="45">
+        <v>45974</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -2953,7 +2993,9 @@
       <c r="M18" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="45">
+        <v>45974</v>
+      </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -3007,7 +3049,9 @@
       <c r="M19" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="45">
+        <v>45974</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -3061,7 +3105,9 @@
       <c r="M20" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="45">
+        <v>45974</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -3115,7 +3161,9 @@
       <c r="M21" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="45">
+        <v>45974</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -3169,7 +3217,9 @@
       <c r="M22" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="45">
+        <v>45974</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -3223,7 +3273,9 @@
       <c r="M23" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="45">
+        <v>45974</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -3277,7 +3329,9 @@
       <c r="M24" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="45">
+        <v>45974</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -3331,7 +3385,9 @@
       <c r="M25" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="45">
+        <v>45974</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -3385,7 +3441,9 @@
       <c r="M26" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="N26" s="1"/>
+      <c r="N26" s="45">
+        <v>45974</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -3439,7 +3497,9 @@
       <c r="M27" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="45">
+        <v>45974</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -3493,7 +3553,9 @@
       <c r="M28" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="N28" s="1"/>
+      <c r="N28" s="45">
+        <v>45974</v>
+      </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -3545,7 +3607,9 @@
       <c r="M29" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="N29" s="1"/>
+      <c r="N29" s="45">
+        <v>45974</v>
+      </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -3599,7 +3663,9 @@
       <c r="M30" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="N30" s="1"/>
+      <c r="N30" s="45">
+        <v>45974</v>
+      </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -3653,7 +3719,9 @@
       <c r="M31" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="N31" s="1"/>
+      <c r="N31" s="45">
+        <v>45974</v>
+      </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -3707,7 +3775,9 @@
       <c r="M32" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="N32" s="1"/>
+      <c r="N32" s="45">
+        <v>45974</v>
+      </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -3761,7 +3831,9 @@
       <c r="M33" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="N33" s="1"/>
+      <c r="N33" s="45">
+        <v>45974</v>
+      </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
@@ -3815,7 +3887,9 @@
       <c r="M34" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="N34" s="1"/>
+      <c r="N34" s="45">
+        <v>45974</v>
+      </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -3869,7 +3943,9 @@
       <c r="M35" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="N35" s="1"/>
+      <c r="N35" s="45">
+        <v>45974</v>
+      </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -3923,7 +3999,9 @@
       <c r="M36" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="N36" s="1"/>
+      <c r="N36" s="45">
+        <v>45974</v>
+      </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -3977,7 +4055,9 @@
       <c r="M37" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="N37" s="1"/>
+      <c r="N37" s="45">
+        <v>45974</v>
+      </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -4031,7 +4111,9 @@
       <c r="M38" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="N38" s="1"/>
+      <c r="N38" s="45">
+        <v>45974</v>
+      </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -4085,7 +4167,9 @@
       <c r="M39" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="N39" s="1"/>
+      <c r="N39" s="45">
+        <v>45974</v>
+      </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -4139,7 +4223,9 @@
       <c r="M40" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="N40" s="1"/>
+      <c r="N40" s="45">
+        <v>45974</v>
+      </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -4193,7 +4279,9 @@
       <c r="M41" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="N41" s="1"/>
+      <c r="N41" s="45">
+        <v>45974</v>
+      </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
@@ -4247,7 +4335,9 @@
       <c r="M42" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="N42" s="1"/>
+      <c r="N42" s="45">
+        <v>45974</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>

</xml_diff>